<commit_message>
- Added Alter Script for Product table, (Added Column for product have variant as boolean type)
</commit_message>
<xml_diff>
--- a/OIMS5/Miscellaneous/ITEM MASTER .xlsx
+++ b/OIMS5/Miscellaneous/ITEM MASTER .xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -549,8 +549,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -587,6 +587,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -633,7 +641,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,9 +673,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -699,6 +708,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -874,25 +884,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="3" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
     <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -901,7 +914,7 @@
     <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -984,7 +997,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1064,7 +1077,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1144,7 +1157,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1224,7 +1237,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1304,7 +1317,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1384,7 +1397,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1464,7 +1477,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1544,7 +1557,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1624,7 +1637,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1704,7 +1717,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1784,7 +1797,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1864,7 +1877,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1944,7 +1957,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2024,7 +2037,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2104,7 +2117,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2184,7 +2197,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2264,7 +2277,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2344,7 +2357,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2424,7 +2437,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2504,7 +2517,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2584,7 +2597,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2664,7 +2677,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2744,7 +2757,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2824,7 +2837,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2904,7 +2917,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2984,7 +2997,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3064,7 +3077,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3144,7 +3157,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3224,7 +3237,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3304,7 +3317,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3384,7 +3397,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3464,7 +3477,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3544,7 +3557,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3624,7 +3637,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3704,7 +3717,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3784,7 +3797,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3864,7 +3877,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3944,7 +3957,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4024,7 +4037,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4104,7 +4117,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4184,7 +4197,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4264,7 +4277,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4344,7 +4357,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4424,7 +4437,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4504,7 +4517,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4584,7 +4597,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4664,7 +4677,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4744,7 +4757,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4824,7 +4837,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4904,7 +4917,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4984,7 +4997,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5064,7 +5077,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5144,7 +5157,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5224,7 +5237,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5304,7 +5317,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5384,7 +5397,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5464,7 +5477,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="58" spans="1:27">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5544,7 +5557,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="59" spans="1:27">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5624,7 +5637,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="60" spans="1:27">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5704,7 +5717,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="61" spans="1:27">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5784,7 +5797,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="62" spans="1:27">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5864,7 +5877,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="63" spans="1:27">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5944,7 +5957,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="64" spans="1:27">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6024,7 +6037,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="65" spans="1:27">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6104,7 +6117,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="66" spans="1:27">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6184,7 +6197,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="67" spans="1:27">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6264,7 +6277,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="68" spans="1:27">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6344,7 +6357,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="69" spans="1:27">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6424,7 +6437,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="70" spans="1:27">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6504,7 +6517,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="71" spans="1:27">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6584,7 +6597,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="72" spans="1:27">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6664,7 +6677,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6744,7 +6757,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="74" spans="1:27">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6824,7 +6837,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="75" spans="1:27">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6904,7 +6917,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="76" spans="1:27">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6984,7 +6997,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="77" spans="1:27">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7064,7 +7077,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="78" spans="1:27">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -7144,7 +7157,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="79" spans="1:27">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7224,7 +7237,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="80" spans="1:27">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7304,7 +7317,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7384,7 +7397,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7464,7 +7477,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7544,7 +7557,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7624,7 +7637,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7704,7 +7717,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -7784,7 +7797,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -7864,7 +7877,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -7944,7 +7957,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8024,7 +8037,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8104,7 +8117,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8184,7 +8197,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8264,7 +8277,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8344,7 +8357,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8424,7 +8437,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8504,7 +8517,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8584,7 +8597,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="97" spans="1:27">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8664,7 +8677,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="98" spans="1:27">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8744,7 +8757,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="99" spans="1:27">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8824,7 +8837,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="100" spans="1:27">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -8904,7 +8917,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="101" spans="1:27">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -8984,7 +8997,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="102" spans="1:27">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -9064,7 +9077,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="103" spans="1:27">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -9144,7 +9157,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="104" spans="1:27">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -9224,7 +9237,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="105" spans="1:27">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -9304,7 +9317,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="106" spans="1:27">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -9384,7 +9397,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="107" spans="1:27">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -9464,7 +9477,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="108" spans="1:27">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -9544,7 +9557,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="109" spans="1:27">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -9624,7 +9637,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="110" spans="1:27">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -9704,7 +9717,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="111" spans="1:27">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -9784,7 +9797,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="112" spans="1:27">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9864,7 +9877,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="113" spans="1:27">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9944,7 +9957,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="114" spans="1:27">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -10024,7 +10037,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="115" spans="1:27">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -10104,7 +10117,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="116" spans="1:27">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -10184,7 +10197,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="117" spans="1:27">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -10264,7 +10277,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="118" spans="1:27">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -10350,24 +10363,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>